<commit_message>
Added trade network example
</commit_message>
<xml_diff>
--- a/data/countries.xlsx
+++ b/data/countries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme 2.0\Business &amp; Projects\Computing\European_System\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91475F7E-78C8-4D40-A00E-15F1BBE159F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D7F4DE-9498-4BD3-8164-D1EF25462D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3043" yWindow="3043" windowWidth="19562" windowHeight="10257" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Greece</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>#ff00ab</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Czechia</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -646,27 +646,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5">
         <v>2.5499999999999998</v>
@@ -677,13 +677,13 @@
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="4">
         <v>-0.31</v>
@@ -694,13 +694,13 @@
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="4">
         <v>2.46</v>
@@ -711,13 +711,13 @@
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4">
         <v>-1.1200000000000001</v>
@@ -728,13 +728,13 @@
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="4">
         <v>-1.72</v>
@@ -745,13 +745,13 @@
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="4">
         <v>0.1</v>
@@ -762,13 +762,13 @@
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" s="4">
         <v>-1.8</v>
@@ -779,13 +779,13 @@
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="4">
         <v>0.65</v>
@@ -796,13 +796,13 @@
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D10" s="4">
         <v>2.04</v>
@@ -813,13 +813,13 @@
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="4">
         <v>1.4</v>
@@ -830,13 +830,13 @@
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="4">
         <v>-0.88</v>
@@ -847,13 +847,13 @@
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="4">
         <v>-0.98</v>
@@ -864,13 +864,13 @@
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4">
         <v>1.25</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="4">
         <v>0.23</v>
@@ -898,13 +898,13 @@
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" s="4">
         <v>0.18</v>
@@ -915,13 +915,13 @@
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" s="4">
         <v>-2.27</v>
@@ -932,13 +932,13 @@
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D18" s="4">
         <v>0.74</v>
@@ -949,13 +949,13 @@
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="4">
         <v>1.67</v>
@@ -966,13 +966,13 @@
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4">
         <v>0.3</v>
@@ -983,13 +983,13 @@
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" s="4">
         <v>-0.52</v>
@@ -1000,13 +1000,13 @@
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22" s="4">
         <v>1.5</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="4">
         <v>0.98</v>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4">
         <v>-0.5</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="4">
         <v>1.34</v>
@@ -1068,13 +1068,13 @@
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26" s="4">
         <v>0.76</v>
@@ -1085,13 +1085,13 @@
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27" s="4">
         <v>-0.62</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28" s="4">
         <v>-2.4500000000000002</v>
@@ -1120,10 +1120,10 @@
     <row r="29" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">
       <c r="C30" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1" ht="13.6" x14ac:dyDescent="0.25">

</xml_diff>